<commit_message>
adicionado formulas e somas
</commit_message>
<xml_diff>
--- a/REFERENCIAS/B3 negociacao-2022-05-02-16-18-56.xlsx
+++ b/REFERENCIAS/B3 negociacao-2022-05-02-16-18-56.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29868" windowHeight="13464"/>
+    <workbookView windowWidth="12660" windowHeight="8004"/>
   </bookViews>
   <sheets>
     <sheet name="Negociação" sheetId="1" r:id="rId1"/>
+    <sheet name="média ponderada" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="76">
   <si>
     <t>Data do Negócio</t>
   </si>
@@ -230,6 +231,18 @@
   </si>
   <si>
     <t>VALE S.A.</t>
+  </si>
+  <si>
+    <t>19/10/2021</t>
+  </si>
+  <si>
+    <t>20/10/2021</t>
+  </si>
+  <si>
+    <t>21/10/2021</t>
+  </si>
+  <si>
+    <t>22/10/2021</t>
   </si>
 </sst>
 </file>
@@ -243,7 +256,7 @@
     <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="_-\R\$* #,##0.00######_-;\-\R\$* #,##0.00######_-;_ \-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -252,17 +265,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Segoe UI"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -409,7 +429,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,18 +438,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.35"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor theme="4" tint="0.799981688894314"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -615,12 +647,23 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.399975585192419"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.399975585192419"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -724,91 +767,85 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -817,10 +854,10 @@
     <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -829,10 +866,10 @@
     <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -841,10 +878,10 @@
     <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -853,10 +890,10 @@
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -865,13 +902,35 @@
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="180" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="180" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -879,15 +938,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="58" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1231,13 +1290,13 @@
   <sheetPr/>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.2222222222222" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="25.3333333333333" customWidth="1"/>
     <col min="3" max="3" width="18.2222222222222" customWidth="1"/>
     <col min="4" max="4" width="35.4444444444444" customWidth="1"/>
@@ -1250,39 +1309,39 @@
   </cols>
   <sheetData>
     <row r="1" ht="16.8" spans="1:10">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
@@ -1297,13 +1356,14 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="11">
         <v>6</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="12">
         <v>28.21</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="13">
+        <f>F2*G2</f>
         <v>169.26</v>
       </c>
       <c r="I2" t="s">
@@ -1314,7 +1374,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
@@ -1329,13 +1389,13 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="11">
         <v>35</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="12">
         <v>13.48</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="13">
         <v>471.8</v>
       </c>
       <c r="I3" t="s">
@@ -1346,7 +1406,7 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
@@ -1361,13 +1421,13 @@
       <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="11">
         <v>20</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="12">
         <v>8.6</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="13">
         <v>172</v>
       </c>
       <c r="I4" t="s">
@@ -1378,7 +1438,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B5" t="s">
@@ -1393,13 +1453,13 @@
       <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="11">
         <v>20</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="12">
         <v>6.14</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="13">
         <v>122.8</v>
       </c>
       <c r="I5" t="s">
@@ -1410,7 +1470,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
@@ -1425,13 +1485,13 @@
       <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="11">
         <v>8</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="12">
         <v>14.12</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="13">
         <v>112.96</v>
       </c>
       <c r="I6" t="s">
@@ -1442,7 +1502,7 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B7" t="s">
@@ -1457,13 +1517,13 @@
       <c r="E7" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="11">
         <v>10</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="12">
         <v>19.75</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="13">
         <v>197.5</v>
       </c>
       <c r="I7" t="s">
@@ -1474,7 +1534,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -1489,13 +1549,13 @@
       <c r="E8" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="11">
         <v>16</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="12">
         <v>27.32</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="13">
         <v>437.12</v>
       </c>
       <c r="I8" t="s">
@@ -1506,7 +1566,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
@@ -1521,13 +1581,13 @@
       <c r="E9" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="11">
         <v>6</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="12">
         <v>28.1</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="13">
         <v>168.6</v>
       </c>
       <c r="I9" t="s">
@@ -1538,7 +1598,7 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B10" t="s">
@@ -1553,13 +1613,13 @@
       <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="11">
         <v>5</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="12">
         <v>82.68</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="13">
         <v>413.4</v>
       </c>
       <c r="I10" t="s">
@@ -1570,7 +1630,7 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B11" t="s">
@@ -1585,13 +1645,13 @@
       <c r="E11" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="11">
         <v>5</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="12">
         <v>22.62</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="13">
         <v>113.1</v>
       </c>
       <c r="I11" t="s">
@@ -1602,7 +1662,7 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B12" t="s">
@@ -1617,13 +1677,13 @@
       <c r="E12" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="11">
         <v>8</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="12">
         <v>10.55</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="13">
         <v>84.4</v>
       </c>
       <c r="I12" t="s">
@@ -1634,7 +1694,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
@@ -1649,13 +1709,13 @@
       <c r="E13" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="11">
         <v>100</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="12">
         <v>1.46</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="13">
         <v>146</v>
       </c>
       <c r="I13" t="s">
@@ -1666,7 +1726,7 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B14" t="s">
@@ -1681,13 +1741,13 @@
       <c r="E14" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="11">
         <v>100</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="12">
         <v>2.17</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="13">
         <v>217</v>
       </c>
       <c r="I14" t="s">
@@ -1698,7 +1758,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B15" t="s">
@@ -1713,13 +1773,13 @@
       <c r="E15" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="11">
         <v>14</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="12">
         <v>3.58</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="13">
         <v>50.12</v>
       </c>
       <c r="I15" t="s">
@@ -1730,7 +1790,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B16" t="s">
@@ -1745,13 +1805,13 @@
       <c r="E16" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="11">
         <v>10</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="12">
         <v>18.59</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="13">
         <v>185.9</v>
       </c>
       <c r="I16" t="s">
@@ -1762,7 +1822,7 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
@@ -1777,13 +1837,13 @@
       <c r="E17" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="11">
         <v>15</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="12">
         <v>36.94</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="13">
         <v>554.1</v>
       </c>
       <c r="I17" t="s">
@@ -1794,7 +1854,7 @@
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B18" t="s">
@@ -1809,13 +1869,13 @@
       <c r="E18" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="11">
         <v>12</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="12">
         <v>85.77</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="13">
         <v>1029.24</v>
       </c>
       <c r="I18" t="s">
@@ -1826,130 +1886,134 @@
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="6">
-        <v>44489</v>
-      </c>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="16">
         <v>4</v>
       </c>
-      <c r="G19" s="9">
-        <v>28.21</v>
-      </c>
-      <c r="H19" s="9">
-        <v>169.26</v>
-      </c>
-      <c r="I19" s="7" t="s">
+      <c r="G19" s="17">
+        <v>30.21</v>
+      </c>
+      <c r="H19" s="17">
+        <f>F19*G19</f>
+        <v>120.84</v>
+      </c>
+      <c r="I19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="J19" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="6">
-        <v>44489</v>
-      </c>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="16">
         <v>5</v>
       </c>
-      <c r="G20" s="9">
-        <v>28.21</v>
-      </c>
-      <c r="H20" s="9">
-        <v>169.26</v>
-      </c>
-      <c r="I20" s="7" t="s">
+      <c r="G20" s="17">
+        <v>28.35</v>
+      </c>
+      <c r="H20" s="17">
+        <f>F20*G20</f>
+        <v>141.75</v>
+      </c>
+      <c r="I20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="J20" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="6">
-        <v>44489</v>
-      </c>
-      <c r="B21" s="7" t="s">
+      <c r="A21" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="16">
         <v>5</v>
       </c>
-      <c r="G21" s="9">
-        <v>28.21</v>
-      </c>
-      <c r="H21" s="9">
-        <v>169.26</v>
-      </c>
-      <c r="I21" s="7" t="s">
+      <c r="G21" s="17">
+        <v>32.06</v>
+      </c>
+      <c r="H21" s="17">
+        <f>F21*G21</f>
+        <v>160.3</v>
+      </c>
+      <c r="I21" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J21" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="6">
-        <v>44489</v>
-      </c>
-      <c r="B22" s="7" t="s">
+      <c r="A22" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="16">
         <v>10</v>
       </c>
-      <c r="G22" s="9">
-        <v>28.21</v>
-      </c>
-      <c r="H22" s="9">
-        <v>169.26</v>
-      </c>
-      <c r="I22" s="7" t="s">
+      <c r="G22" s="17">
+        <v>25</v>
+      </c>
+      <c r="H22" s="17">
+        <f>F22*G22</f>
+        <v>250</v>
+      </c>
+      <c r="I22" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="15" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1961,4 +2025,112 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="13.8" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="4" width="8.88888888888889" style="1"/>
+    <col min="5" max="5" width="9.11111111111111" style="1"/>
+    <col min="6" max="16384" width="8.88888888888889" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="3:3">
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="14.4" spans="3:5">
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4">
+        <v>28.21</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="14.4" spans="3:5">
+      <c r="C6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="7">
+        <v>30.21</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="14.4" spans="3:5">
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6">
+        <v>5</v>
+      </c>
+      <c r="E7" s="7">
+        <v>28.35</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="14.4" spans="3:5">
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="6">
+        <v>5</v>
+      </c>
+      <c r="E8" s="7">
+        <v>32.06</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="14.4" spans="3:5">
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="6">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="2:8">
+      <c r="B14" s="8">
+        <f>((28.21*6)+(30.21*4)+(28.35*5)+(32.06*5)+(25*10))/(6+4+5+5+10)</f>
+        <v>28.0716666666667</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" s="8">
+        <f>((28.21*6)+(30.21*4)+(28.35*5)+(32.06*5)+(25*10))</f>
+        <v>842.15</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="C18:G18"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>